<commit_message>
new figs and text updates
</commit_message>
<xml_diff>
--- a/SupportingInformation.xlsx
+++ b/SupportingInformation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Trendlines" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="83">
   <si>
     <t>Case</t>
   </si>
@@ -34,7 +34,7 @@
     <t>All</t>
   </si>
   <si>
-    <t>Y = 7229269.334096*X^-1.95517449</t>
+    <t>Y =6015004.7659681*X^-1.9292826071</t>
   </si>
   <si>
     <t>Energy Efficiency</t>
@@ -43,22 +43,22 @@
     <t>AA uptake w/ &amp; w/o synthesis</t>
   </si>
   <si>
-    <t>Y = -0.0164666944*X+89.2348988418</t>
+    <t>Y = -0.0165286577*X + 90.956655699</t>
   </si>
   <si>
     <t>AA synthesis w/o uptake</t>
   </si>
   <si>
-    <t>Y= -0.00310715*X+32.75368345</t>
+    <t>Y= -0.0031763617*X+33.475197551</t>
   </si>
   <si>
     <t>Carbon Yield</t>
   </si>
   <si>
-    <t>Y = -0.0080654408*X+63.540138</t>
-  </si>
-  <si>
-    <t>Y = -0.0069488777*X+57.8526085978</t>
+    <t>Y = -0.0080291315*X + 63.8261160855</t>
+  </si>
+  <si>
+    <t>Y = -0.0069792882*X+58.8562299</t>
   </si>
   <si>
     <t>* CAT productivity was excluded from the trendline</t>
@@ -67,6 +67,60 @@
     <t>X = Carbon number of protein</t>
   </si>
   <si>
+    <t>Carbon Number</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>w/o Syn</t>
+  </si>
+  <si>
+    <t>w/o AA</t>
+  </si>
+  <si>
+    <t>experiment</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>BMP10</t>
+  </si>
+  <si>
+    <t>CASP9</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>deGFP</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>FGF21</t>
+  </si>
+  <si>
+    <t>scFvR4</t>
+  </si>
+  <si>
+    <t>CAT (sigma70)</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
     <t>Transcription Stoichiometric Coefficient</t>
   </si>
   <si>
@@ -82,28 +136,7 @@
     <t>UTP</t>
   </si>
   <si>
-    <t>BMP10</t>
-  </si>
-  <si>
-    <t>CAT</t>
-  </si>
-  <si>
     <t>dCas9</t>
-  </si>
-  <si>
-    <t>deGFP</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>F10</t>
-  </si>
-  <si>
-    <t>FGF21</t>
-  </si>
-  <si>
-    <t>scFvR4</t>
   </si>
   <si>
     <t>Protein</t>
@@ -242,7 +275,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -266,6 +299,13 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -314,8 +354,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -323,8 +367,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -344,10 +392,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -358,13 +406,13 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -375,10 +423,10 @@
       <c r="B2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" s="2" t="n">
         <v>0.99</v>
       </c>
     </row>
@@ -389,22 +437,22 @@
       <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="n">
-        <v>0.97</v>
+      <c r="F3" s="2" t="n">
+        <v>0.91</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="1" t="n">
-        <v>0.79</v>
+      <c r="F4" s="2" t="n">
+        <v>0.78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -414,22 +462,22 @@
       <c r="B5" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>0.92</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="0" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.83</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -440,6 +488,895 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>2123</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>45.2</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>44.8</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>43.1</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>47.2</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>46.7</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J13" s="0" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>1175</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>51.6</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="H14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>1140</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>56.6</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>55.1</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>51.8</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>3066</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>38.4</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>2376</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>45.8</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>44.1</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>42.4</v>
+      </c>
+      <c r="H17" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J17" s="0" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>992</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>55.7</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>54.7</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>52.9</v>
+      </c>
+      <c r="H18" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>1230</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>51.9</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>50.9</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>48.2</v>
+      </c>
+      <c r="H19" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4"/>
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>58</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>56.9</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>51.8</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J20" s="0" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I22" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>2123</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="J24" s="0" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K24" s="0" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>1175</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <v>11.4</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="K25" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="L25" s="0" t="n">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>1140</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K26" s="0" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>3066</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="E27" s="0" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="K27" s="0" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>2376</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="E28" s="0" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J28" s="0" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="K28" s="0" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>992</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>9.8</v>
+      </c>
+      <c r="E29" s="0" t="n">
+        <v>9.7</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="K29" s="0" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>1230</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="H30" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="K30" s="0" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>8.7</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>2123</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>55.8</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>53.6</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>28.2</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>2004</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>55.9</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>53.3</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>26.2</v>
+      </c>
+      <c r="H35" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="J35" s="0" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="K35" s="0" t="n">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>1175</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>77.3</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>71.3</v>
+      </c>
+      <c r="E36" s="0" t="n">
+        <v>27.6</v>
+      </c>
+      <c r="F36" s="0" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="J36" s="0" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="K36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L36" s="0" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>1140</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>74.4</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>69.7</v>
+      </c>
+      <c r="E37" s="0" t="n">
+        <v>29.3</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="J37" s="0" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="K37" s="0" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>3066</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>43.7</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>41.5</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <v>23.6</v>
+      </c>
+      <c r="H38" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="J38" s="0" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="K38" s="0" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>2376</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>55.2</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>48.5</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <v>25.8</v>
+      </c>
+      <c r="H39" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="J39" s="0" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="K39" s="0" t="n">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>992</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>82.4</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>73.1</v>
+      </c>
+      <c r="E40" s="0" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="H40" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="J40" s="0" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="K40" s="0" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>1230</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>65.8</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <v>30.4</v>
+      </c>
+      <c r="H41" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="K41" s="0" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>76.6</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>70.1</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>27.7</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -470,214 +1407,214 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="n">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="n">
         <v>445</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>360</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="2" t="n">
         <v>397</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" s="2" t="n">
         <v>381</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" s="2" t="n">
         <v>424</v>
       </c>
-      <c r="G3" s="1" t="n">
+      <c r="G3" s="2" t="n">
         <v>848</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="n">
+      <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="2" t="n">
         <v>176</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>144</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="2" t="n">
         <v>151</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" s="2" t="n">
         <v>189</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" s="2" t="n">
         <v>219</v>
       </c>
-      <c r="G4" s="1" t="n">
+      <c r="G4" s="2" t="n">
         <v>438</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="1" t="n">
+      <c r="A5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="2" t="n">
         <v>259</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>339</v>
       </c>
-      <c r="D5" s="1" t="n">
+      <c r="D5" s="2" t="n">
         <v>365</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" s="2" t="n">
         <v>288</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="2" t="n">
         <v>416</v>
       </c>
-      <c r="G5" s="1" t="n">
+      <c r="G5" s="2" t="n">
         <v>832</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="1" t="n">
+      <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="n">
         <v>163</v>
       </c>
-      <c r="C6" s="1" t="n">
+      <c r="C6" s="2" t="n">
         <v>231</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="D6" s="2" t="n">
         <v>183</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="2" t="n">
         <v>101</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="2" t="n">
         <v>225</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="2" t="n">
         <v>450</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="1" t="n">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2" t="n">
         <v>480</v>
       </c>
-      <c r="C7" s="1" t="n">
+      <c r="C7" s="2" t="n">
         <v>549</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="2" t="n">
         <v>633</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>394</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="2" t="n">
         <v>622</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="2" t="n">
         <v>1244</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="1" t="n">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="n">
         <v>403</v>
       </c>
-      <c r="C8" s="1" t="n">
+      <c r="C8" s="2" t="n">
         <v>450</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="D8" s="2" t="n">
         <v>460</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="2" t="n">
         <v>246</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" s="2" t="n">
         <v>488</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="2" t="n">
         <v>976</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="1" t="n">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="n">
         <v>110</v>
       </c>
-      <c r="C9" s="1" t="n">
+      <c r="C9" s="2" t="n">
         <v>193</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="D9" s="2" t="n">
         <v>222</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="2" t="n">
         <v>105</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" s="2" t="n">
         <v>209</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="2" t="n">
         <v>418</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="n">
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>180</v>
       </c>
-      <c r="C10" s="1" t="n">
+      <c r="C10" s="2" t="n">
         <v>221</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="D10" s="2" t="n">
         <v>281</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="2" t="n">
         <v>134</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" s="2" t="n">
         <v>271</v>
       </c>
-      <c r="G10" s="1" t="n">
+      <c r="G10" s="2" t="n">
         <v>542</v>
       </c>
     </row>
@@ -722,19 +1659,19 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>29</v>
+      <c r="A1" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,49 +1763,49 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>33</v>
+      <c r="A12" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,49 +2055,49 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
-        <v>40</v>
+      <c r="A21" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F22" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="0" t="s">
-        <v>32</v>
-      </c>
       <c r="H22" s="0" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1534,43 +2471,43 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,43 +2881,43 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="L44" s="0" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="M44" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2353,49 +3290,49 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="2" t="s">
-        <v>59</v>
+      <c r="A55" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="K56" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="L56" s="0" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="M56" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2728,43 +3665,43 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="K66" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="L66" s="0" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="M66" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
new energy efficiency text and updated figs
</commit_message>
<xml_diff>
--- a/SupportingInformation.xlsx
+++ b/SupportingInformation.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="88">
   <si>
     <t xml:space="preserve">Case</t>
   </si>
@@ -54,13 +54,13 @@
     <t xml:space="preserve">AA uptake w/ &amp; w/o synthesis</t>
   </si>
   <si>
-    <t xml:space="preserve">Y = -0.0165286577*X + 90.956655699</t>
+    <t xml:space="preserve">Y = -0.0004013838*X+86.1952399977</t>
   </si>
   <si>
     <t xml:space="preserve">AA synthesis w/o uptake</t>
   </si>
   <si>
-    <t xml:space="preserve">Y= -0.0031763617*X+33.475197551</t>
+    <t xml:space="preserve">Y= -0.0030272199*X+67.3997545927</t>
   </si>
   <si>
     <t xml:space="preserve">Carbon Yield</t>
@@ -84,21 +84,24 @@
     <t xml:space="preserve">Yield</t>
   </si>
   <si>
+    <t xml:space="preserve">AA w/ Syn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w/o Syn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w/o AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error</t>
+  </si>
+  <si>
     <t xml:space="preserve">Control</t>
   </si>
   <si>
-    <t xml:space="preserve">w/o Syn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w/o AA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">experiment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Error</t>
-  </si>
-  <si>
     <t xml:space="preserve">BMP10</t>
   </si>
   <si>
@@ -126,13 +129,19 @@
     <t xml:space="preserve">CAT (sigma70)</t>
   </si>
   <si>
+    <t xml:space="preserve">MBP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Productivity</t>
   </si>
   <si>
     <t xml:space="preserve">Efficiency</t>
   </si>
   <si>
-    <t xml:space="preserve">Transcription Stoichiometric Coefficient</t>
+    <t xml:space="preserve">Transcription stoichiometric coefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Translation stoichiometric coefficient</t>
   </si>
   <si>
     <t xml:space="preserve">ATP</t>
@@ -383,7 +392,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -403,17 +412,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4132653061224"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.4591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.1428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.0510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,7 +474,7 @@
         <v>10</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>0.91</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -480,7 +488,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>0.78</v>
+        <v>0.65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,7 +552,7 @@
         <v>24</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J12" s="0" t="s">
         <v>21</v>
@@ -561,7 +569,7 @@
         <v>2123</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>45.2</v>
@@ -573,7 +581,7 @@
         <v>43.1</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I13" s="0" t="n">
         <v>3.9</v>
@@ -590,7 +598,7 @@
         <v>2004</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>47.2</v>
@@ -602,7 +610,7 @@
         <v>44</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I14" s="0" t="n">
         <v>3.1</v>
@@ -619,7 +627,7 @@
         <v>1175</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>58.2</v>
@@ -634,7 +642,7 @@
         <v>6.2</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I15" s="0" t="n">
         <v>2.3</v>
@@ -654,7 +662,7 @@
         <v>1140</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>56.6</v>
@@ -666,7 +674,7 @@
         <v>51.8</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I16" s="0" t="n">
         <v>2.4</v>
@@ -683,7 +691,7 @@
         <v>3066</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>40.7</v>
@@ -695,7 +703,7 @@
         <v>38.4</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I17" s="0" t="n">
         <v>3.9</v>
@@ -712,7 +720,7 @@
         <v>2376</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>45.8</v>
@@ -724,7 +732,7 @@
         <v>42.4</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I18" s="0" t="n">
         <v>3</v>
@@ -741,7 +749,7 @@
         <v>992</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>55.7</v>
@@ -753,7 +761,7 @@
         <v>52.9</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I19" s="0" t="n">
         <v>2.2</v>
@@ -770,7 +778,7 @@
         <v>1230</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>51.9</v>
@@ -782,7 +790,7 @@
         <v>48.2</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I20" s="0" t="n">
         <v>2.9</v>
@@ -795,9 +803,11 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4"/>
+      <c r="A21" s="4" t="n">
+        <v>1175</v>
+      </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>58</v>
@@ -809,7 +819,7 @@
         <v>51.8</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I21" s="0" t="n">
         <v>2.5</v>
@@ -822,78 +832,75 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A22" s="4" t="n">
+        <v>1419</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>50.7</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>50.2</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <v>46.8</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="J22" s="0" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="0" t="s">
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E24" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J23" s="0" t="s">
+      <c r="I24" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="K23" s="0" t="s">
+      <c r="K24" s="0" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>2123</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="0" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D24" s="0" t="n">
-        <v>2.4</v>
-      </c>
-      <c r="E24" s="0" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="K24" s="0" t="n">
-        <v>0.7</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>2004</v>
+        <v>2123</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>26</v>
       </c>
       <c r="C25" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D25" s="0" t="n">
         <v>2.4</v>
-      </c>
-      <c r="D25" s="0" t="n">
-        <v>2.5</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>2.5</v>
@@ -913,501 +920,594 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>1175</v>
+        <v>2004</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>27</v>
       </c>
       <c r="C26" s="0" t="n">
-        <v>12</v>
+        <v>2.4</v>
       </c>
       <c r="D26" s="0" t="n">
-        <v>11.8</v>
+        <v>2.5</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>11.4</v>
-      </c>
-      <c r="F26" s="0" t="n">
-        <v>11.6</v>
+        <v>2.5</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>27</v>
       </c>
       <c r="I26" s="0" t="n">
-        <v>2.9</v>
+        <v>0.7</v>
       </c>
       <c r="J26" s="0" t="n">
-        <v>3.1</v>
+        <v>0.7</v>
       </c>
       <c r="K26" s="0" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="L26" s="0" t="n">
-        <v>3.5</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>1140</v>
+        <v>1175</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>28</v>
       </c>
       <c r="C27" s="0" t="n">
-        <v>8.3</v>
+        <v>11.5</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>8.4</v>
+        <v>11.4</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>8.2</v>
+        <v>11.4</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <v>11.6</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>28</v>
       </c>
       <c r="I27" s="0" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="J27" s="0" t="n">
-        <v>2</v>
+        <v>3.3</v>
       </c>
       <c r="K27" s="0" t="n">
-        <v>2.4</v>
+        <v>2.9</v>
+      </c>
+      <c r="L27" s="0" t="n">
+        <v>3.5</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>3066</v>
+        <v>1140</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>29</v>
       </c>
       <c r="C28" s="0" t="n">
-        <v>1.1</v>
+        <v>8.3</v>
       </c>
       <c r="D28" s="0" t="n">
-        <v>1.1</v>
+        <v>8.4</v>
       </c>
       <c r="E28" s="0" t="n">
-        <v>1.1</v>
+        <v>8.2</v>
       </c>
       <c r="H28" s="0" t="s">
         <v>29</v>
       </c>
       <c r="I28" s="0" t="n">
-        <v>0.3</v>
+        <v>2.5</v>
       </c>
       <c r="J28" s="0" t="n">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="K28" s="0" t="n">
-        <v>0.3</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
-        <v>2376</v>
+        <v>3066</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>30</v>
       </c>
       <c r="C29" s="0" t="n">
-        <v>1.9</v>
+        <v>1.1</v>
       </c>
       <c r="D29" s="0" t="n">
-        <v>1.9</v>
+        <v>1.1</v>
       </c>
       <c r="E29" s="0" t="n">
-        <v>1.8</v>
+        <v>1.1</v>
       </c>
       <c r="H29" s="0" t="s">
         <v>30</v>
       </c>
       <c r="I29" s="0" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="J29" s="0" t="n">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="K29" s="0" t="n">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
-        <v>992</v>
+        <v>2376</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>31</v>
       </c>
       <c r="C30" s="0" t="n">
-        <v>10</v>
+        <v>1.9</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>9.8</v>
+        <v>1.9</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>9.7</v>
+        <v>1.8</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>31</v>
       </c>
       <c r="I30" s="0" t="n">
-        <v>3.1</v>
+        <v>0.5</v>
       </c>
       <c r="J30" s="0" t="n">
-        <v>2.6</v>
+        <v>0.6</v>
       </c>
       <c r="K30" s="0" t="n">
-        <v>2.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>1230</v>
+        <v>992</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>32</v>
       </c>
       <c r="C31" s="0" t="n">
-        <v>6.2</v>
+        <v>10</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>5.9</v>
+        <v>9.8</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>5.9</v>
+        <v>9.7</v>
       </c>
       <c r="H31" s="0" t="s">
         <v>32</v>
       </c>
       <c r="I31" s="0" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="K31" s="0" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>1230</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I32" s="0" t="n">
         <v>1.7</v>
       </c>
-      <c r="J31" s="0" t="n">
+      <c r="J32" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="K31" s="0" t="n">
+      <c r="K32" s="0" t="n">
         <v>1.4</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="0" t="n">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>1175</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="0" t="n">
         <v>8.8</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D33" s="0" t="n">
         <v>8.7</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E33" s="0" t="n">
         <v>8.9</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I32" s="0" t="n">
+      <c r="H33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" s="0" t="n">
         <v>2.3</v>
       </c>
-      <c r="J32" s="0" t="n">
+      <c r="J33" s="0" t="n">
         <v>2.3</v>
       </c>
-      <c r="K32" s="0" t="n">
+      <c r="K33" s="0" t="n">
         <v>2.3</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="0" t="n">
+        <v>1419</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="J34" s="0" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="K34" s="0" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="0" t="s">
+      <c r="B36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D36" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E34" s="0" t="s">
+      <c r="E36" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H36" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I34" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="J34" s="0" t="s">
+      <c r="I36" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="K34" s="0" t="s">
+      <c r="K36" s="0" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>2123</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C35" s="0" t="n">
-        <v>55.8</v>
-      </c>
-      <c r="D35" s="0" t="n">
-        <v>53.6</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>28.2</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" s="0" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="J35" s="0" t="n">
-        <v>7.4</v>
-      </c>
-      <c r="K35" s="0" t="n">
-        <v>2.2</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <v>2004</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="0" t="n">
-        <v>55.9</v>
-      </c>
-      <c r="D36" s="0" t="n">
-        <v>53.3</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>26.2</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="I36" s="0" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="J36" s="0" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="K36" s="0" t="n">
-        <v>1.8</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>1175</v>
+        <v>2123</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C37" s="0" t="n">
-        <v>77.3</v>
+        <v>83.9</v>
       </c>
       <c r="D37" s="0" t="n">
-        <v>71.3</v>
+        <v>83.3</v>
       </c>
       <c r="E37" s="0" t="n">
-        <v>27.6</v>
-      </c>
-      <c r="F37" s="0" t="n">
-        <v>3.6</v>
+        <v>74.4</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I37" s="0" t="n">
-        <v>7.3</v>
+        <v>0.1</v>
       </c>
       <c r="J37" s="0" t="n">
-        <v>6.4</v>
+        <v>0</v>
       </c>
       <c r="K37" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L37" s="0" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
-        <v>1140</v>
+        <v>2004</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C38" s="0" t="n">
-        <v>74.4</v>
+        <v>84.2</v>
       </c>
       <c r="D38" s="0" t="n">
-        <v>69.7</v>
+        <v>83.3</v>
       </c>
       <c r="E38" s="0" t="n">
-        <v>29.3</v>
+        <v>74.6</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I38" s="0" t="n">
-        <v>7.2</v>
+        <v>0.1</v>
       </c>
       <c r="J38" s="0" t="n">
-        <v>6.4</v>
+        <v>0</v>
       </c>
       <c r="K38" s="0" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
-        <v>3066</v>
+        <v>1175</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C39" s="0" t="n">
-        <v>43.7</v>
+        <v>84.2</v>
       </c>
       <c r="D39" s="0" t="n">
-        <v>41.5</v>
+        <v>83.3</v>
       </c>
       <c r="E39" s="0" t="n">
-        <v>23.6</v>
+        <v>68</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <v>13.3</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I39" s="0" t="n">
-        <v>7.1</v>
+        <v>0.1</v>
       </c>
       <c r="J39" s="0" t="n">
-        <v>6.3</v>
+        <v>0</v>
       </c>
       <c r="K39" s="0" t="n">
-        <v>2.2</v>
+        <v>1.2</v>
+      </c>
+      <c r="L39" s="0" t="n">
+        <v>4.7</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>2376</v>
+        <v>1140</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C40" s="0" t="n">
-        <v>55.2</v>
+        <v>84</v>
       </c>
       <c r="D40" s="0" t="n">
-        <v>48.5</v>
+        <v>83.3</v>
       </c>
       <c r="E40" s="0" t="n">
-        <v>25.8</v>
+        <v>69.5</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I40" s="0" t="n">
-        <v>7.1</v>
+        <v>0.1</v>
       </c>
       <c r="J40" s="0" t="n">
-        <v>7.2</v>
+        <v>0</v>
       </c>
       <c r="K40" s="0" t="n">
-        <v>1.7</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
-        <v>992</v>
+        <v>3066</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" s="0" t="n">
-        <v>82.4</v>
+        <v>84</v>
       </c>
       <c r="D41" s="0" t="n">
-        <v>73.1</v>
+        <v>83.3</v>
       </c>
       <c r="E41" s="0" t="n">
-        <v>31.9</v>
+        <v>75.8</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I41" s="0" t="n">
-        <v>7.8</v>
+        <v>0.1</v>
       </c>
       <c r="J41" s="0" t="n">
-        <v>6.7</v>
+        <v>0</v>
       </c>
       <c r="K41" s="0" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
+        <v>2376</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42" s="0" t="n">
+        <v>84.6</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="H42" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" s="0" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>992</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" s="0" t="n">
+        <v>84.9</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="E43" s="0" t="n">
+        <v>72.6</v>
+      </c>
+      <c r="H43" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K43" s="0" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
         <v>1230</v>
       </c>
-      <c r="B42" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="0" t="n">
-        <v>67.5</v>
-      </c>
-      <c r="D42" s="0" t="n">
-        <v>65.8</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>30.4</v>
-      </c>
-      <c r="H42" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="I42" s="0" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="J42" s="0" t="n">
-        <v>7.1</v>
-      </c>
-      <c r="K42" s="0" t="n">
-        <v>1.4</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="3" t="s">
+      <c r="B44" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="0" t="n">
-        <v>76.6</v>
-      </c>
-      <c r="D43" s="0" t="n">
-        <v>70.1</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>27.7</v>
-      </c>
-      <c r="H43" s="3" t="s">
+      <c r="C44" s="0" t="n">
+        <v>83.6</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="H44" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="I43" s="0" t="n">
-        <v>7.7</v>
-      </c>
-      <c r="J43" s="0" t="n">
-        <v>6.4</v>
-      </c>
-      <c r="K43" s="0" t="n">
+      <c r="I44" s="0" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K44" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>1175</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="0" t="n">
+        <v>84.2</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K45" s="0" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>1419</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="0" t="n">
+        <v>84.7</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="E46" s="0" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="H46" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="0" t="n">
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
@@ -1426,48 +1526,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="1" sqref="A7 C29"/>
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>445</v>
@@ -1490,7 +1587,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>176</v>
@@ -1513,7 +1610,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>259</v>
@@ -1536,7 +1633,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>163</v>
@@ -1559,7 +1656,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>480</v>
@@ -1582,7 +1679,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>403</v>
@@ -1605,7 +1702,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" s="2" t="n">
         <v>110</v>
@@ -1628,7 +1725,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>180</v>
@@ -1647,6 +1744,30 @@
       </c>
       <c r="G10" s="2" t="n">
         <v>542</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>238</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>264</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>228</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>191</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <f aca="false">35+5+14+14+1+9+16+20+1+10+33+19+6+8+25+29+27+1+7+26</f>
+        <v>306</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>612</v>
       </c>
     </row>
   </sheetData>
@@ -1668,41 +1789,40 @@
   <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O67" activeCellId="1" sqref="A7 O67"/>
+      <selection pane="topLeft" activeCell="O67" activeCellId="0" sqref="O67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.58673469387755"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,48 +1915,48 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D13" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="F13" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2087,48 +2207,48 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2502,43 +2622,43 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J33" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="K33" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L33" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="M33" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2912,43 +3032,43 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J44" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K44" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L44" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="M44" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3322,48 +3442,48 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J56" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="K56" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L56" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="M56" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3696,43 +3816,43 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J66" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K66" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L66" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="M66" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>